<commit_message>
Range slider added to about page
</commit_message>
<xml_diff>
--- a/Sample Companies Financials Database Format.xlsx
+++ b/Sample Companies Financials Database Format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3708a04485001ab/Platform/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="803" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD84643-A1A3-4EC3-8CF7-40DDF82FABB0}"/>
+  <xr:revisionPtr revIDLastSave="805" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8492057-9098-4B01-B6F7-AC16295EC416}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
   </bookViews>
@@ -556,9 +556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384203C-F021-4178-95D6-38ABC9D05E39}">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4532,6 +4534,12 @@
         <v>0.43897108271687962</v>
       </c>
     </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D63" s="1">
+        <f>MAX(D2:D61)</f>
+        <v>16025000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Filter to query only 2023 data included
</commit_message>
<xml_diff>
--- a/Sample Companies Financials Database Format.xlsx
+++ b/Sample Companies Financials Database Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3708a04485001ab/Platform/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="805" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8492057-9098-4B01-B6F7-AC16295EC416}"/>
+  <xr:revisionPtr revIDLastSave="809" documentId="8_{B5691506-39FA-424E-99D4-26D7CBA25480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C965506B-8972-4194-9568-0E881C15A118}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3D767867-0467-441D-9DC3-18181976D26B}"/>
   </bookViews>
@@ -556,11 +556,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384203C-F021-4178-95D6-38ABC9D05E39}">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,7 +687,7 @@
         <v>-3.3374157991426824E-2</v>
       </c>
       <c r="Q2" s="7">
-        <v>0.56774193548387097</v>
+        <v>-0.56774193548387097</v>
       </c>
       <c r="R2" s="7">
         <v>-7.1856287425149698E-2</v>
@@ -754,7 +752,7 @@
         <v>-5.2098408104196817E-2</v>
       </c>
       <c r="Q3" s="7">
-        <v>0.6257309941520468</v>
+        <v>-0.6257309941520468</v>
       </c>
       <c r="R3" s="7">
         <v>-0.15258148254975484</v>
@@ -819,7 +817,7 @@
         <v>1.2054794520547946E-2</v>
       </c>
       <c r="Q4" s="7">
-        <v>0.40645161290322579</v>
+        <v>-0.40645161290322579</v>
       </c>
       <c r="R4" s="7">
         <v>-6.7534294759057339E-2</v>
@@ -884,7 +882,7 @@
         <v>-0.58611111111111114</v>
       </c>
       <c r="Q5" s="7">
-        <v>2.4563106796116503</v>
+        <v>-2.4563106796116503</v>
       </c>
       <c r="R5" s="7">
         <v>-0.14991055456171734</v>
@@ -1014,7 +1012,7 @@
         <v>8.4619782732990284E-2</v>
       </c>
       <c r="Q7" s="7">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="R7" s="7">
         <v>6.5331928345626969E-2</v>
@@ -1079,7 +1077,7 @@
         <v>9.4004944375772559E-2</v>
       </c>
       <c r="Q8" s="7">
-        <v>-7.4444444444444446</v>
+        <v>7.4444444444444446</v>
       </c>
       <c r="R8" s="7">
         <v>7.0742799393633149E-2</v>
@@ -1144,7 +1142,7 @@
         <v>0.1096797153024911</v>
       </c>
       <c r="Q9" s="7">
-        <v>-6.2222222222222223</v>
+        <v>6.2222222222222223</v>
       </c>
       <c r="R9" s="7">
         <v>5.5940023068050751E-2</v>
@@ -1209,7 +1207,7 @@
         <v>7.7407932011331448E-2</v>
       </c>
       <c r="Q10" s="7">
-        <v>-4.6190476190476186</v>
+        <v>4.6190476190476186</v>
       </c>
       <c r="R10" s="7">
         <v>5.584950029394474E-2</v>
@@ -1274,7 +1272,7 @@
         <v>6.3171521035598699E-2</v>
       </c>
       <c r="Q11" s="7">
-        <v>-12.818181818181818</v>
+        <v>12.818181818181818</v>
       </c>
       <c r="R11" s="7">
         <v>4.6524985640436528E-2</v>
@@ -1339,7 +1337,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="Q12" s="7">
-        <v>-3.588888888888889</v>
+        <v>3.588888888888889</v>
       </c>
       <c r="R12" s="7">
         <v>-0.12521109770808203</v>
@@ -1404,7 +1402,7 @@
         <v>0.59466019417475724</v>
       </c>
       <c r="Q13" s="7">
-        <v>-2.8452380952380953</v>
+        <v>2.8452380952380953</v>
       </c>
       <c r="R13" s="7">
         <v>9.7174571140262359E-2</v>
@@ -1469,7 +1467,7 @@
         <v>0.31837606837606836</v>
       </c>
       <c r="Q14" s="7">
-        <v>-2.4301075268817205</v>
+        <v>2.4301075268817205</v>
       </c>
       <c r="R14" s="7">
         <v>-0.11616901408450704</v>
@@ -1534,7 +1532,7 @@
         <v>0.61074918566775249</v>
       </c>
       <c r="Q15" s="7">
-        <v>-2.9680851063829787</v>
+        <v>2.9680851063829787</v>
       </c>
       <c r="R15" s="7">
         <v>-9.1329479768786123E-2</v>
@@ -1599,7 +1597,7 @@
         <v>0.67809734513274333</v>
       </c>
       <c r="Q16" s="7">
-        <v>-2.2109375</v>
+        <v>2.2109375</v>
       </c>
       <c r="R16" s="7">
         <v>-2.3743472584856398E-2</v>
@@ -1664,7 +1662,7 @@
         <v>0.46843754868627252</v>
       </c>
       <c r="Q17" s="7">
-        <v>-90.550420168067234</v>
+        <v>90.550420168067234</v>
       </c>
       <c r="R17" s="7">
         <v>0.29049510937373585</v>
@@ -1729,7 +1727,7 @@
         <v>0.2745366103743126</v>
       </c>
       <c r="Q18" s="7">
-        <v>-76.770833333333329</v>
+        <v>76.770833333333329</v>
       </c>
       <c r="R18" s="7">
         <v>0.28193728962829806</v>
@@ -1794,7 +1792,7 @@
         <v>0.31940806166252933</v>
       </c>
       <c r="Q19" s="7">
-        <v>-71.14556962025317</v>
+        <v>71.14556962025317</v>
       </c>
       <c r="R19" s="7">
         <v>0.26993797007533527</v>
@@ -1859,7 +1857,7 @@
         <v>0.30778941056734177</v>
       </c>
       <c r="Q20" s="7">
-        <v>-58.0625</v>
+        <v>58.0625</v>
       </c>
       <c r="R20" s="7">
         <v>0.27462920919179273</v>
@@ -1924,7 +1922,7 @@
         <v>0.29996568225581971</v>
       </c>
       <c r="Q21" s="7">
-        <v>-912.35714285714289</v>
+        <v>912.35714285714289</v>
       </c>
       <c r="R21" s="7">
         <v>0.29386194210475358</v>
@@ -1989,7 +1987,7 @@
         <v>0.13327449249779347</v>
       </c>
       <c r="Q22" s="7">
-        <v>-3.9680851063829787</v>
+        <v>3.9680851063829787</v>
       </c>
       <c r="R22" s="7">
         <v>0.22439024390243903</v>
@@ -2054,7 +2052,7 @@
         <v>0.1162751957354656</v>
       </c>
       <c r="Q23" s="7">
-        <v>-4.2541666666666664</v>
+        <v>4.2541666666666664</v>
       </c>
       <c r="R23" s="7">
         <v>0.15671211830228537</v>
@@ -2119,7 +2117,7 @@
         <v>0.18562767475035663</v>
       </c>
       <c r="Q24" s="7">
-        <v>-5.5340314136125652</v>
+        <v>5.5340314136125652</v>
       </c>
       <c r="R24" s="7">
         <v>0.17375478927203064</v>
@@ -2184,7 +2182,7 @@
         <v>0.19065531577905365</v>
       </c>
       <c r="Q25" s="7">
-        <v>-4.5162790697674415</v>
+        <v>4.5162790697674415</v>
       </c>
       <c r="R25" s="7">
         <v>0.14116852414724756</v>
@@ -2249,7 +2247,7 @@
         <v>8.1447963800904979E-2</v>
       </c>
       <c r="Q26" s="7">
-        <v>-17.731343283582088</v>
+        <v>17.731343283582088</v>
       </c>
       <c r="R26" s="7">
         <v>0.19666572478101157</v>
@@ -2314,7 +2312,7 @@
         <v>9.6265836684311365E-2</v>
       </c>
       <c r="Q27" s="7">
-        <v>-57.920634920634917</v>
+        <v>57.920634920634917</v>
       </c>
       <c r="R27" s="7">
         <v>6.4243620542472069E-2</v>
@@ -2379,7 +2377,7 @@
         <v>0.15450002172873842</v>
       </c>
       <c r="Q28" s="7">
-        <v>-53.957805907172997</v>
+        <v>53.957805907172997</v>
       </c>
       <c r="R28" s="7">
         <v>5.8395018617949983E-2</v>
@@ -2444,7 +2442,7 @@
         <v>0.12509722582317864</v>
       </c>
       <c r="Q29" s="7">
-        <v>-31.915397631133672</v>
+        <v>31.915397631133672</v>
       </c>
       <c r="R29" s="7">
         <v>5.2852132105248945E-2</v>
@@ -2509,7 +2507,7 @@
         <v>9.4242252967340817E-2</v>
       </c>
       <c r="Q30" s="7">
-        <v>-28.816161616161615</v>
+        <v>28.816161616161615</v>
       </c>
       <c r="R30" s="7">
         <v>4.5708191869069381E-2</v>
@@ -2571,7 +2569,7 @@
         <v>8.9870235248556973E-2</v>
       </c>
       <c r="Q31" s="7">
-        <v>-395.21212121212119</v>
+        <v>395.21212121212119</v>
       </c>
       <c r="R31" s="7">
         <v>4.4651436794097339E-2</v>
@@ -2636,7 +2634,7 @@
         <v>3.2099999999999997E-2</v>
       </c>
       <c r="Q32" s="7">
-        <v>-10.052631578947368</v>
+        <v>10.052631578947368</v>
       </c>
       <c r="R32" s="7">
         <v>0.12996171670360668</v>
@@ -2831,7 +2829,7 @@
         <v>0.15252976190476192</v>
       </c>
       <c r="Q35" s="7">
-        <v>-3.6904761904761907</v>
+        <v>3.6904761904761907</v>
       </c>
       <c r="R35" s="7">
         <v>0.11424219345011424</v>
@@ -2896,7 +2894,7 @@
         <v>8.9867841409691632E-2</v>
       </c>
       <c r="Q36" s="7">
-        <v>-1.8717948717948718</v>
+        <v>1.8717948717948718</v>
       </c>
       <c r="R36" s="7">
         <v>3.7760995113282986E-2</v>
@@ -2961,7 +2959,7 @@
         <v>0.38041631265930331</v>
       </c>
       <c r="Q37" s="7">
-        <v>-194.77777777777777</v>
+        <v>194.77777777777777</v>
       </c>
       <c r="R37" s="7">
         <v>0.41217870257037942</v>
@@ -3026,7 +3024,7 @@
         <v>0.25241080038572805</v>
       </c>
       <c r="Q38" s="7">
-        <v>-199.125</v>
+        <v>199.125</v>
       </c>
       <c r="R38" s="7">
         <v>0.3998754282155092</v>
@@ -3220,7 +3218,9 @@
       <c r="P41" s="7">
         <v>0.22966473609952684</v>
       </c>
-      <c r="Q41" s="7"/>
+      <c r="Q41" s="7">
+        <v>0</v>
+      </c>
       <c r="R41" s="7">
         <v>0.47841982846343944</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>2.0005274957140974E-2</v>
       </c>
       <c r="Q42" s="7">
-        <v>-24.625</v>
+        <v>24.625</v>
       </c>
       <c r="R42" s="7">
         <v>7.2478991596638662E-2</v>
@@ -3349,7 +3349,7 @@
         <v>2.4146304446805281E-2</v>
       </c>
       <c r="Q43" s="7">
-        <v>-42.8</v>
+        <v>42.8</v>
       </c>
       <c r="R43" s="7">
         <v>7.4145402022147325E-2</v>
@@ -3414,7 +3414,7 @@
         <v>-7.2592067988668559E-4</v>
       </c>
       <c r="Q44" s="7">
-        <v>-15.166666666666666</v>
+        <v>15.166666666666666</v>
       </c>
       <c r="R44" s="7">
         <v>3.3084311632870865E-2</v>
@@ -3479,7 +3479,7 @@
         <v>5.7908937605396289E-2</v>
       </c>
       <c r="Q45" s="7">
-        <v>-19.285714285714285</v>
+        <v>19.285714285714285</v>
       </c>
       <c r="R45" s="7">
         <v>2.4742268041237112E-2</v>
@@ -3544,7 +3544,7 @@
         <v>2.5152363696260914E-2</v>
       </c>
       <c r="Q46" s="7">
-        <v>-83</v>
+        <v>83</v>
       </c>
       <c r="R46" s="7">
         <v>0.10778443113772455</v>
@@ -3609,7 +3609,7 @@
         <v>-1.7605503660318499E-2</v>
       </c>
       <c r="Q47" s="7">
-        <v>-11.136580007323325</v>
+        <v>11.136580007323325</v>
       </c>
       <c r="R47" s="7">
         <v>2.7922479982923003E-2</v>
@@ -3674,7 +3674,7 @@
         <v>0.12414844624341471</v>
       </c>
       <c r="Q48" s="7">
-        <v>-21.750274544256534</v>
+        <v>21.750274544256534</v>
       </c>
       <c r="R48" s="7">
         <v>0.11393556743604333</v>
@@ -3739,7 +3739,7 @@
         <v>0.15059610038761206</v>
       </c>
       <c r="Q49" s="7">
-        <v>-10.447841105354058</v>
+        <v>10.447841105354058</v>
       </c>
       <c r="R49" s="7">
         <v>4.2072729629183896E-2</v>
@@ -3804,7 +3804,7 @@
         <v>6.4793846387409385E-2</v>
       </c>
       <c r="Q50" s="7">
-        <v>-2.9826224328593995</v>
+        <v>2.9826224328593995</v>
       </c>
       <c r="R50" s="7">
         <v>-4.1218445552258919E-2</v>
@@ -3869,7 +3869,7 @@
         <v>9.1521953198112682E-2</v>
       </c>
       <c r="Q51" s="7">
-        <v>-19.419522571496099</v>
+        <v>19.419522571496099</v>
       </c>
       <c r="R51" s="7">
         <v>8.621036236235198E-2</v>
@@ -3934,7 +3934,7 @@
         <v>0.49282560706401768</v>
       </c>
       <c r="Q52" s="7">
-        <v>-5.17741935483871</v>
+        <v>5.17741935483871</v>
       </c>
       <c r="R52" s="7">
         <v>5.0107372942018613E-2</v>
@@ -3999,7 +3999,7 @@
         <v>0.48873390557939916</v>
       </c>
       <c r="Q53" s="7">
-        <v>-15.605263157894736</v>
+        <v>15.605263157894736</v>
       </c>
       <c r="R53" s="7">
         <v>9.5642458100558658E-2</v>
@@ -4064,7 +4064,7 @@
         <v>0.4286128004633652</v>
       </c>
       <c r="Q54" s="7">
-        <v>-11.620689655172415</v>
+        <v>11.620689655172415</v>
       </c>
       <c r="R54" s="7">
         <v>8.9150943396226409E-2</v>
@@ -4129,7 +4129,7 @@
         <v>0.40345199568500539</v>
       </c>
       <c r="Q55" s="7">
-        <v>-11.390243902439025</v>
+        <v>11.390243902439025</v>
       </c>
       <c r="R55" s="7">
         <v>7.2097141411586144E-2</v>
@@ -4194,7 +4194,7 @@
         <v>0.25634824667472794</v>
       </c>
       <c r="Q56" s="7">
-        <v>-7.8354430379746836</v>
+        <v>7.8354430379746836</v>
       </c>
       <c r="R56" s="7">
         <v>0.13256726457399104</v>
@@ -4259,7 +4259,7 @@
         <v>-1.875041853612804E-3</v>
       </c>
       <c r="Q57" s="7">
-        <v>-5.6111111111111107</v>
+        <v>5.6111111111111107</v>
       </c>
       <c r="R57" s="7">
         <v>3.7558685446009391E-2</v>
@@ -4324,7 +4324,7 @@
         <v>1.0483619344773791E-2</v>
       </c>
       <c r="Q58" s="7">
-        <v>-6.1341463414634143</v>
+        <v>6.1341463414634143</v>
       </c>
       <c r="R58" s="7">
         <v>1.74017401740174E-2</v>
@@ -4454,7 +4454,7 @@
         <v>1.1525005145091582E-2</v>
       </c>
       <c r="Q60" s="7">
-        <v>-2.7684210526315791</v>
+        <v>2.7684210526315791</v>
       </c>
       <c r="R60" s="7">
         <v>3.4642032332563508E-2</v>
@@ -4519,7 +4519,7 @@
         <v>6.7007910656119128E-3</v>
       </c>
       <c r="Q61" s="7">
-        <v>-5.1226415094339623</v>
+        <v>5.1226415094339623</v>
       </c>
       <c r="R61" s="7">
         <v>6.9435104236718226E-2</v>
@@ -4532,12 +4532,6 @@
       </c>
       <c r="U61" s="7">
         <v>0.43897108271687962</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D63" s="1">
-        <f>MAX(D2:D61)</f>
-        <v>16025000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added firms' financials criteria data sourcing and comparison to range slider values
</commit_message>
<xml_diff>
--- a/Sample Companies Financials Database Format.xlsx
+++ b/Sample Companies Financials Database Format.xlsx
@@ -558,7 +558,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C384203C-F021-4178-95D6-38ABC9D05E39}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>